<commit_message>
export date functions to Excel (41/1114)
</commit_message>
<xml_diff>
--- a/UnitTests/Tests/Utilities.xlsx
+++ b/UnitTests/Tests/Utilities.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>Function</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>Actual</t>
-  </si>
-  <si>
-    <t>1.8.1</t>
   </si>
   <si>
     <t>1.8.2</t>
@@ -458,11 +455,11 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="4" t="str">
         <f>IF(B3=C3,"PASS","FAIL")</f>
-        <v>FAIL</v>
+        <v>PASS</v>
       </c>
       <c r="E3" t="str">
         <f>_xll.qlVersion()</f>

</xml_diff>